<commit_message>
Patran ha dejado de funcionar
</commit_message>
<xml_diff>
--- a/Satelite/Satelite.xlsx
+++ b/Satelite/Satelite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Andres\1_Universidad\MUSE\EUE\Practica2_EUE\Satelite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F70B8A-5CD3-420B-95C9-3E266E6E666E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A64A8E-C01A-419C-B8E6-5F7D4CB3E1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="61">
   <si>
     <t>Elemento</t>
   </si>
@@ -230,6 +230,15 @@
   </si>
   <si>
     <t>Tensor de tensiones</t>
+  </si>
+  <si>
+    <t>Random Z 1.251885E+02</t>
+  </si>
+  <si>
+    <t>Random Y 7.093872E+01</t>
+  </si>
+  <si>
+    <t>Random X 7.093872E+01</t>
   </si>
 </sst>
 </file>
@@ -524,9 +533,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,6 +545,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -546,18 +555,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -584,11 +581,44 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -696,7 +726,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="C8C8C8"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -953,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="M112" sqref="M112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,10 +1050,10 @@
       <c r="M1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="58" t="s">
+      <c r="N1" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="59"/>
+      <c r="O1" s="55"/>
       <c r="P1" s="15" t="s">
         <v>9</v>
       </c>
@@ -1074,7 +1104,7 @@
         <f t="array" aca="1" ref="J2" ca="1">1/((D2*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C2*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.89542760593648674</v>
       </c>
-      <c r="L2" s="63" t="s">
+      <c r="L2" s="59" t="s">
         <v>36</v>
       </c>
       <c r="M2" s="51" t="s">
@@ -1191,7 +1221,7 @@
         <f t="array" aca="1" ref="J3" ca="1">1/((D3*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C3*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.90275098885523397</v>
       </c>
-      <c r="L3" s="64"/>
+      <c r="L3" s="60"/>
       <c r="M3" s="51"/>
       <c r="N3" s="13" t="s">
         <v>23</v>
@@ -1286,7 +1316,7 @@
         <f t="array" aca="1" ref="J4" ca="1">1/((D4*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C4*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.88788997095129907</v>
       </c>
-      <c r="L4" s="65"/>
+      <c r="L4" s="61"/>
       <c r="M4" s="51"/>
       <c r="N4" s="13" t="s">
         <v>24</v>
@@ -1381,10 +1411,10 @@
         <f t="array" aca="1" ref="J5" ca="1">1/((D5*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C5*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>0.83282435452232617</v>
       </c>
-      <c r="L5" s="63" t="s">
+      <c r="L5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="63" t="s">
+      <c r="M5" s="59" t="s">
         <v>39</v>
       </c>
       <c r="N5" s="37" t="s">
@@ -1498,8 +1528,8 @@
         <f t="array" aca="1" ref="J6" ca="1">1/((D6*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C6*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.59045912696254055</v>
       </c>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
       <c r="N6" s="37" t="s">
         <v>23</v>
       </c>
@@ -1557,8 +1587,8 @@
         <f t="array" aca="1" ref="J7" ca="1">1/((D7*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C7*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.58974855289360728</v>
       </c>
-      <c r="L7" s="64"/>
-      <c r="M7" s="65"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="61"/>
       <c r="N7" s="37" t="s">
         <v>24</v>
       </c>
@@ -1616,8 +1646,8 @@
         <f t="array" aca="1" ref="J8" ca="1">1/((D8*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C8*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>0.52307734265045136</v>
       </c>
-      <c r="L8" s="64"/>
-      <c r="M8" s="63" t="s">
+      <c r="L8" s="60"/>
+      <c r="M8" s="59" t="s">
         <v>40</v>
       </c>
       <c r="N8" s="37" t="s">
@@ -1677,8 +1707,8 @@
         <f t="array" aca="1" ref="J9" ca="1">1/((D9*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C9*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.88791678786750927</v>
       </c>
-      <c r="L9" s="64"/>
-      <c r="M9" s="64"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
       <c r="N9" s="37" t="s">
         <v>23</v>
       </c>
@@ -1736,8 +1766,8 @@
         <f t="array" aca="1" ref="J10" ca="1">1/((D10*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C10*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.90276591520375382</v>
       </c>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
       <c r="N10" s="37" t="s">
         <v>24</v>
       </c>
@@ -2837,10 +2867,10 @@
       <c r="M40" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="N40" s="54" t="s">
+      <c r="N40" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="O40" s="55"/>
+      <c r="O40" s="63"/>
       <c r="P40" s="18" t="s">
         <v>9</v>
       </c>
@@ -2855,7 +2885,7 @@
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="50" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="19">
@@ -2891,10 +2921,10 @@
         <f t="array" aca="1" ref="J41" ca="1">1/((D41*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C41*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.96064736465470835</v>
       </c>
-      <c r="L41" s="60" t="s">
+      <c r="L41" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="M41" s="46" t="s">
+      <c r="M41" s="50" t="s">
         <v>57</v>
       </c>
       <c r="N41" s="19" t="s">
@@ -2920,7 +2950,7 @@
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A42" s="46"/>
+      <c r="A42" s="50"/>
       <c r="B42" s="19">
         <v>40240</v>
       </c>
@@ -2954,8 +2984,8 @@
         <f t="array" aca="1" ref="J42" ca="1">1/((D42*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C42*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.96823175895535873</v>
       </c>
-      <c r="L42" s="61"/>
-      <c r="M42" s="46"/>
+      <c r="L42" s="57"/>
+      <c r="M42" s="50"/>
       <c r="N42" s="19" t="s">
         <v>23</v>
       </c>
@@ -2975,7 +3005,7 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A43" s="46"/>
+      <c r="A43" s="50"/>
       <c r="B43" s="19">
         <v>40250</v>
       </c>
@@ -3009,8 +3039,8 @@
         <f t="array" aca="1" ref="J43" ca="1">1/((D43*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C43*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.98381191987101102</v>
       </c>
-      <c r="L43" s="62"/>
-      <c r="M43" s="46"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="50"/>
       <c r="N43" s="19" t="s">
         <v>24</v>
       </c>
@@ -3030,7 +3060,7 @@
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A44" s="46"/>
+      <c r="A44" s="50"/>
       <c r="B44" s="19">
         <v>40360</v>
       </c>
@@ -3064,10 +3094,10 @@
         <f t="array" aca="1" ref="J44" ca="1">1/((D44*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C44*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>0.83282435452232617</v>
       </c>
-      <c r="L44" s="60" t="s">
+      <c r="L44" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="M44" s="60" t="s">
+      <c r="M44" s="56" t="s">
         <v>39</v>
       </c>
       <c r="N44" s="36" t="s">
@@ -3093,7 +3123,7 @@
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A45" s="46"/>
+      <c r="A45" s="50"/>
       <c r="B45" s="19">
         <v>40390</v>
       </c>
@@ -3127,8 +3157,8 @@
         <f t="array" aca="1" ref="J45" ca="1">1/((D45*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C45*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.90044472096336314</v>
       </c>
-      <c r="L45" s="61"/>
-      <c r="M45" s="61"/>
+      <c r="L45" s="57"/>
+      <c r="M45" s="57"/>
       <c r="N45" s="36" t="s">
         <v>23</v>
       </c>
@@ -3148,7 +3178,7 @@
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" s="46"/>
+      <c r="A46" s="50"/>
       <c r="B46" s="19">
         <v>40710</v>
       </c>
@@ -3182,8 +3212,8 @@
         <f t="array" aca="1" ref="J46" ca="1">1/((D46*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C46*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.90046884492425372</v>
       </c>
-      <c r="L46" s="61"/>
-      <c r="M46" s="62"/>
+      <c r="L46" s="57"/>
+      <c r="M46" s="58"/>
       <c r="N46" s="36" t="s">
         <v>24</v>
       </c>
@@ -3203,7 +3233,7 @@
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" s="46"/>
+      <c r="A47" s="50"/>
       <c r="B47" s="19">
         <v>40740</v>
       </c>
@@ -3237,8 +3267,8 @@
         <f t="array" aca="1" ref="J47" ca="1">1/((D47*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C47*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.98250307302451168</v>
       </c>
-      <c r="L47" s="61"/>
-      <c r="M47" s="60" t="s">
+      <c r="L47" s="57"/>
+      <c r="M47" s="56" t="s">
         <v>40</v>
       </c>
       <c r="N47" s="36" t="s">
@@ -3260,7 +3290,7 @@
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A48" s="46"/>
+      <c r="A48" s="50"/>
       <c r="B48" s="19">
         <v>40750</v>
       </c>
@@ -3294,8 +3324,8 @@
         <f t="array" aca="1" ref="J48" ca="1">1/((D48*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C48*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.98382461077704109</v>
       </c>
-      <c r="L48" s="61"/>
-      <c r="M48" s="61"/>
+      <c r="L48" s="57"/>
+      <c r="M48" s="57"/>
       <c r="N48" s="36" t="s">
         <v>23</v>
       </c>
@@ -3315,7 +3345,7 @@
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" s="46"/>
+      <c r="A49" s="50"/>
       <c r="B49" s="19">
         <v>40760</v>
       </c>
@@ -3349,8 +3379,8 @@
         <f t="array" aca="1" ref="J49" ca="1">1/((D49*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C49*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>-0.96824725392623501</v>
       </c>
-      <c r="L49" s="62"/>
-      <c r="M49" s="62"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="58"/>
       <c r="N49" s="36" t="s">
         <v>24</v>
       </c>
@@ -3370,7 +3400,7 @@
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A50" s="46"/>
+      <c r="A50" s="50"/>
       <c r="B50" s="19">
         <v>40770</v>
       </c>
@@ -3446,7 +3476,7 @@
       <c r="S53"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A54" s="46" t="s">
+      <c r="A54" s="50" t="s">
         <v>31</v>
       </c>
       <c r="B54" s="19">
@@ -3492,7 +3522,7 @@
       <c r="S54"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A55" s="46"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="19">
         <v>40240</v>
       </c>
@@ -3536,7 +3566,7 @@
       <c r="S55"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A56" s="46"/>
+      <c r="A56" s="50"/>
       <c r="B56" s="19">
         <v>40250</v>
       </c>
@@ -3580,7 +3610,7 @@
       <c r="S56"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A57" s="46"/>
+      <c r="A57" s="50"/>
       <c r="B57" s="19">
         <v>40360</v>
       </c>
@@ -3624,7 +3654,7 @@
       <c r="S57"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A58" s="46"/>
+      <c r="A58" s="50"/>
       <c r="B58" s="19">
         <v>40390</v>
       </c>
@@ -3668,7 +3698,7 @@
       <c r="S58"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A59" s="46"/>
+      <c r="A59" s="50"/>
       <c r="B59" s="19">
         <v>40710</v>
       </c>
@@ -3712,7 +3742,7 @@
       <c r="S59"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A60" s="46"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="19">
         <v>40740</v>
       </c>
@@ -3756,7 +3786,7 @@
       <c r="S60"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A61" s="46"/>
+      <c r="A61" s="50"/>
       <c r="B61" s="19">
         <v>40750</v>
       </c>
@@ -3800,7 +3830,7 @@
       <c r="S61"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A62" s="46"/>
+      <c r="A62" s="50"/>
       <c r="B62" s="19">
         <v>40760</v>
       </c>
@@ -3844,7 +3874,7 @@
       <c r="S62"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A63" s="46"/>
+      <c r="A63" s="50"/>
       <c r="B63" s="19">
         <v>40770</v>
       </c>
@@ -3948,7 +3978,7 @@
       <c r="S66"/>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A67" s="46" t="s">
+      <c r="A67" s="50" t="s">
         <v>32</v>
       </c>
       <c r="B67" s="19">
@@ -3990,7 +4020,7 @@
       <c r="S67"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A68" s="46"/>
+      <c r="A68" s="50"/>
       <c r="B68" s="19">
         <v>40240</v>
       </c>
@@ -4030,7 +4060,7 @@
       <c r="S68"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A69" s="46"/>
+      <c r="A69" s="50"/>
       <c r="B69" s="19">
         <v>40250</v>
       </c>
@@ -4070,7 +4100,7 @@
       <c r="S69"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A70" s="46"/>
+      <c r="A70" s="50"/>
       <c r="B70" s="19">
         <v>40360</v>
       </c>
@@ -4110,7 +4140,7 @@
       <c r="S70"/>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A71" s="46"/>
+      <c r="A71" s="50"/>
       <c r="B71" s="19">
         <v>40390</v>
       </c>
@@ -4150,7 +4180,7 @@
       <c r="S71"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A72" s="46"/>
+      <c r="A72" s="50"/>
       <c r="B72" s="19">
         <v>40710</v>
       </c>
@@ -4190,7 +4220,7 @@
       <c r="S72"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A73" s="46"/>
+      <c r="A73" s="50"/>
       <c r="B73" s="19">
         <v>40740</v>
       </c>
@@ -4230,7 +4260,7 @@
       <c r="S73"/>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A74" s="46"/>
+      <c r="A74" s="50"/>
       <c r="B74" s="19">
         <v>40750</v>
       </c>
@@ -4270,7 +4300,7 @@
       <c r="S74"/>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A75" s="46"/>
+      <c r="A75" s="50"/>
       <c r="B75" s="19">
         <v>40760</v>
       </c>
@@ -4310,7 +4340,7 @@
       <c r="S75"/>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A76" s="46"/>
+      <c r="A76" s="50"/>
       <c r="B76" s="19">
         <v>40770</v>
       </c>
@@ -4406,10 +4436,10 @@
       <c r="M79" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="N79" s="56" t="s">
+      <c r="N79" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="O79" s="57"/>
+      <c r="O79" s="65"/>
       <c r="P79" s="22" t="s">
         <v>9</v>
       </c>
@@ -4424,42 +4454,46 @@
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A80" s="47" t="s">
+      <c r="A80" s="46" t="s">
         <v>33</v>
       </c>
       <c r="B80" s="23">
         <v>40230</v>
       </c>
-      <c r="C80" s="23"/>
-      <c r="D80" s="23"/>
+      <c r="C80" s="23">
+        <v>757.39114000000006</v>
+      </c>
+      <c r="D80" s="23">
+        <v>3676.1329074071541</v>
+      </c>
       <c r="E80" s="44" cm="1">
         <f t="array" aca="1" ref="E80" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C80*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58082306867924505</v>
       </c>
       <c r="F80" s="44" cm="1">
         <f t="array" aca="1" ref="F80" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C80*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G80" s="44" t="e" cm="1">
+        <v>0.82946940926799151</v>
+      </c>
+      <c r="G80" s="44" cm="1">
         <f t="array" aca="1" ref="G80" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C80*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H80" s="44" t="e" cm="1">
+        <v>11.981072542978692</v>
+      </c>
+      <c r="H80" s="44" cm="1">
         <f t="array" aca="1" ref="H80" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C80)*INDIRECT(ADDRESS(5,38))/(D80*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.5137440799694859</v>
       </c>
       <c r="I80" s="44" cm="1">
         <f t="array" aca="1" ref="I80" ca="1">1/((D80*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C80*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>0.51840503368384461</v>
       </c>
       <c r="J80" s="44" cm="1">
         <f t="array" aca="1" ref="J80" ca="1">1/((D80*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C80*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="L80" s="47" t="s">
+        <v>0.70290257973980275</v>
+      </c>
+      <c r="L80" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="M80" s="50" t="s">
+      <c r="M80" s="49" t="s">
         <v>57</v>
       </c>
       <c r="N80" s="23" t="s">
@@ -4481,38 +4515,42 @@
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A81" s="48"/>
+      <c r="A81" s="47"/>
       <c r="B81" s="23">
         <v>40240</v>
       </c>
-      <c r="C81" s="23"/>
-      <c r="D81" s="23"/>
+      <c r="C81" s="23">
+        <v>54.757109000000007</v>
+      </c>
+      <c r="D81" s="23">
+        <v>35561238.825024046</v>
+      </c>
       <c r="E81" s="44" cm="1">
         <f t="array" aca="1" ref="E81" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C81*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58274387399495531</v>
       </c>
       <c r="F81" s="44" cm="1">
         <f t="array" aca="1" ref="F81" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C81*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G81" s="44" t="e" cm="1">
+        <v>0.83258138944874971</v>
+      </c>
+      <c r="G81" s="44" cm="1">
         <f t="array" aca="1" ref="G81" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C81*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H81" s="44" t="e" cm="1">
+        <v>178.55201637378866</v>
+      </c>
+      <c r="H81" s="44" cm="1">
         <f t="array" aca="1" ref="H81" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C81)*INDIRECT(ADDRESS(5,38))/(D81*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99994701806116948</v>
       </c>
       <c r="I81" s="44" cm="1">
         <f t="array" aca="1" ref="I81" ca="1">1/((D81*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C81*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.9994358385875074</v>
       </c>
       <c r="J81" s="44" cm="1">
         <f t="array" aca="1" ref="J81" ca="1">1/((D81*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C81*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="L81" s="48"/>
-      <c r="M81" s="50"/>
+        <v>-0.99951834497406922</v>
+      </c>
+      <c r="L81" s="47"/>
+      <c r="M81" s="49"/>
       <c r="N81" s="23" t="s">
         <v>23</v>
       </c>
@@ -4532,38 +4570,42 @@
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A82" s="48"/>
+      <c r="A82" s="47"/>
       <c r="B82" s="23">
         <v>40250</v>
       </c>
-      <c r="C82" s="23"/>
-      <c r="D82" s="23"/>
+      <c r="C82" s="23">
+        <v>140.27937000000003</v>
+      </c>
+      <c r="D82" s="23">
+        <v>81743956.96048671</v>
+      </c>
       <c r="E82" s="44" cm="1">
         <f t="array" aca="1" ref="E82" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C82*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58250983054338001</v>
       </c>
       <c r="F82" s="44" cm="1">
         <f t="array" aca="1" ref="F82" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C82*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G82" s="44" t="e" cm="1">
+        <v>0.83220204386943908</v>
+      </c>
+      <c r="G82" s="44" cm="1">
         <f t="array" aca="1" ref="G82" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C82*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H82" s="44" t="e" cm="1">
+        <v>69.086922487243356</v>
+      </c>
+      <c r="H82" s="44" cm="1">
         <f t="array" aca="1" ref="H82" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C82)*INDIRECT(ADDRESS(5,38))/(D82*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99997709494074394</v>
       </c>
       <c r="I82" s="44" cm="1">
         <f t="array" aca="1" ref="I82" ca="1">1/((D82*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C82*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99975457170774806</v>
       </c>
       <c r="J82" s="44" cm="1">
         <f t="array" aca="1" ref="J82" ca="1">1/((D82*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C82*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="L82" s="49"/>
-      <c r="M82" s="50"/>
+        <v>-0.99979046463463628</v>
+      </c>
+      <c r="L82" s="48"/>
+      <c r="M82" s="49"/>
       <c r="N82" s="23" t="s">
         <v>24</v>
       </c>
@@ -4583,12 +4625,16 @@
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A83" s="48"/>
+      <c r="A83" s="47"/>
       <c r="B83" s="23">
         <v>40360</v>
       </c>
-      <c r="C83" s="23"/>
-      <c r="D83" s="23"/>
+      <c r="C83" s="23">
+        <v>0</v>
+      </c>
+      <c r="D83" s="23">
+        <v>0</v>
+      </c>
       <c r="E83" s="44" cm="1">
         <f t="array" aca="1" ref="E83" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C83*INDIRECT(ADDRESS(5,36)))-1</f>
         <v>0.58289376072382715</v>
@@ -4613,10 +4659,10 @@
         <f t="array" aca="1" ref="J83" ca="1">1/((D83*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C83*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
         <v>0.83282435452232617</v>
       </c>
-      <c r="L83" s="47" t="s">
+      <c r="L83" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="M83" s="47" t="s">
+      <c r="M83" s="46" t="s">
         <v>39</v>
       </c>
       <c r="N83" s="35" t="s">
@@ -4638,38 +4684,42 @@
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A84" s="48"/>
+      <c r="A84" s="47"/>
       <c r="B84" s="23">
         <v>40390</v>
       </c>
-      <c r="C84" s="23"/>
-      <c r="D84" s="23"/>
+      <c r="C84" s="23">
+        <v>158.00565000000003</v>
+      </c>
+      <c r="D84" s="23">
+        <v>2593641.473362511</v>
+      </c>
       <c r="E84" s="44" cm="1">
         <f t="array" aca="1" ref="E84" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C84*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58246132879549384</v>
       </c>
       <c r="F84" s="44" cm="1">
         <f t="array" aca="1" ref="F84" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C84*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G84" s="44" t="e" cm="1">
+        <v>0.83212343620068219</v>
+      </c>
+      <c r="G84" s="44" cm="1">
         <f t="array" aca="1" ref="G84" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C84*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H84" s="44" t="e" cm="1">
+        <v>61.224036493311033</v>
+      </c>
+      <c r="H84" s="44" cm="1">
         <f t="array" aca="1" ref="H84" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C84)*INDIRECT(ADDRESS(5,38))/(D84*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99927903910394866</v>
       </c>
       <c r="I84" s="44" cm="1">
         <f t="array" aca="1" ref="I84" ca="1">1/((D84*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C84*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99226491381549253</v>
       </c>
       <c r="J84" s="44" cm="1">
         <f t="array" aca="1" ref="J84" ca="1">1/((D84*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C84*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="L84" s="48"/>
-      <c r="M84" s="48"/>
+        <v>-0.99339610393086397</v>
+      </c>
+      <c r="L84" s="47"/>
+      <c r="M84" s="47"/>
       <c r="N84" s="35" t="s">
         <v>23</v>
       </c>
@@ -4689,38 +4739,42 @@
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A85" s="48"/>
+      <c r="A85" s="47"/>
       <c r="B85" s="23">
         <v>40710</v>
       </c>
-      <c r="C85" s="23"/>
-      <c r="D85" s="23"/>
+      <c r="C85" s="23">
+        <v>157.80270000000002</v>
+      </c>
+      <c r="D85" s="23">
+        <v>2597627.4440807798</v>
+      </c>
       <c r="E85" s="44" cm="1">
         <f t="array" aca="1" ref="E85" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C85*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58246188408016142</v>
       </c>
       <c r="F85" s="44" cm="1">
         <f t="array" aca="1" ref="F85" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C85*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G85" s="44" t="e" cm="1">
+        <v>0.83212433614978365</v>
+      </c>
+      <c r="G85" s="44" cm="1">
         <f t="array" aca="1" ref="G85" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C85*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H85" s="44" t="e" cm="1">
+        <v>61.304062805955361</v>
+      </c>
+      <c r="H85" s="44" cm="1">
         <f t="array" aca="1" ref="H85" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C85)*INDIRECT(ADDRESS(5,38))/(D85*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99928013465669951</v>
       </c>
       <c r="I85" s="44" cm="1">
         <f t="array" aca="1" ref="I85" ca="1">1/((D85*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C85*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99227678275843045</v>
       </c>
       <c r="J85" s="44" cm="1">
         <f t="array" aca="1" ref="J85" ca="1">1/((D85*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C85*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="L85" s="48"/>
-      <c r="M85" s="49"/>
+        <v>-0.99340623725275223</v>
+      </c>
+      <c r="L85" s="47"/>
+      <c r="M85" s="48"/>
       <c r="N85" s="35" t="s">
         <v>24</v>
       </c>
@@ -4740,38 +4794,42 @@
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A86" s="48"/>
+      <c r="A86" s="47"/>
       <c r="B86" s="23">
         <v>40740</v>
       </c>
-      <c r="C86" s="23"/>
-      <c r="D86" s="23"/>
+      <c r="C86" s="23">
+        <v>807.62264000000005</v>
+      </c>
+      <c r="D86" s="23">
+        <v>113127625.20374614</v>
+      </c>
       <c r="E86" s="44" cm="1">
         <f t="array" aca="1" ref="E86" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C86*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58068592832669852</v>
       </c>
       <c r="F86" s="44" cm="1">
         <f t="array" aca="1" ref="F86" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C86*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G86" s="44" t="e" cm="1">
+        <v>0.8292473377051075</v>
+      </c>
+      <c r="G86" s="44" cm="1">
         <f t="array" aca="1" ref="G86" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C86*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H86" s="44" t="e" cm="1">
+        <v>11.173692074493271</v>
+      </c>
+      <c r="H86" s="44" cm="1">
         <f t="array" aca="1" ref="H86" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C86)*INDIRECT(ADDRESS(5,38))/(D86*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99998425991757045</v>
       </c>
       <c r="I86" s="44" cm="1">
         <f t="array" aca="1" ref="I86" ca="1">1/((D86*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C86*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99982265799500691</v>
       </c>
       <c r="J86" s="44" cm="1">
         <f t="array" aca="1" ref="J86" ca="1">1/((D86*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C86*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="L86" s="48"/>
-      <c r="M86" s="47" t="s">
+        <v>-0.99984859356933831</v>
+      </c>
+      <c r="L86" s="47"/>
+      <c r="M86" s="46" t="s">
         <v>40</v>
       </c>
       <c r="N86" s="35" t="s">
@@ -4793,38 +4851,42 @@
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A87" s="48"/>
+      <c r="A87" s="47"/>
       <c r="B87" s="23">
         <v>40750</v>
       </c>
-      <c r="C87" s="23"/>
-      <c r="D87" s="23"/>
+      <c r="C87" s="23">
+        <v>140.12273000000002</v>
+      </c>
+      <c r="D87" s="23">
+        <v>81846254.329409897</v>
+      </c>
       <c r="E87" s="44" cm="1">
         <f t="array" aca="1" ref="E87" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C87*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58251025914705212</v>
       </c>
       <c r="F87" s="44" cm="1">
         <f t="array" aca="1" ref="F87" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C87*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G87" s="44" t="e" cm="1">
+        <v>0.83220273852382776</v>
+      </c>
+      <c r="G87" s="44" cm="1">
         <f t="array" aca="1" ref="G87" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C87*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H87" s="44" t="e" cm="1">
+        <v>69.16527105737471</v>
+      </c>
+      <c r="H87" s="44" cm="1">
         <f t="array" aca="1" ref="H87" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C87)*INDIRECT(ADDRESS(5,38))/(D87*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99997712330612853</v>
       </c>
       <c r="I87" s="44" cm="1">
         <f t="array" aca="1" ref="I87" ca="1">1/((D87*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C87*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99975487846177313</v>
       </c>
       <c r="J87" s="44" cm="1">
         <f t="array" aca="1" ref="J87" ca="1">1/((D87*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C87*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="L87" s="48"/>
-      <c r="M87" s="48"/>
+        <v>-0.999790726527089</v>
+      </c>
+      <c r="L87" s="47"/>
+      <c r="M87" s="47"/>
       <c r="N87" s="35" t="s">
         <v>23</v>
       </c>
@@ -4844,38 +4906,42 @@
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A88" s="48"/>
+      <c r="A88" s="47"/>
       <c r="B88" s="23">
         <v>40760</v>
       </c>
-      <c r="C88" s="23"/>
-      <c r="D88" s="23"/>
+      <c r="C88" s="23">
+        <v>54.532445000000003</v>
+      </c>
+      <c r="D88" s="23">
+        <v>35594548.06547533</v>
+      </c>
       <c r="E88" s="44" cm="1">
         <f t="array" aca="1" ref="E88" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C88*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.5827444889101161</v>
       </c>
       <c r="F88" s="44" cm="1">
         <f t="array" aca="1" ref="F88" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C88*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G88" s="44" t="e" cm="1">
+        <v>0.83258238618323666</v>
+      </c>
+      <c r="G88" s="44" cm="1">
         <f t="array" aca="1" ref="G88" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C88*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H88" s="44" t="e" cm="1">
+        <v>179.29173883088009</v>
+      </c>
+      <c r="H88" s="44" cm="1">
         <f t="array" aca="1" ref="H88" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C88)*INDIRECT(ADDRESS(5,38))/(D88*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99994706677404777</v>
       </c>
       <c r="I88" s="44" cm="1">
         <f t="array" aca="1" ref="I88" ca="1">1/((D88*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C88*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99943636652750889</v>
       </c>
       <c r="J88" s="44" cm="1">
         <f t="array" aca="1" ref="J88" ca="1">1/((D88*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C88*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="L88" s="49"/>
-      <c r="M88" s="49"/>
+        <v>-0.99951879570494895</v>
+      </c>
+      <c r="L88" s="48"/>
+      <c r="M88" s="48"/>
       <c r="N88" s="35" t="s">
         <v>24</v>
       </c>
@@ -4895,12 +4961,16 @@
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A89" s="49"/>
+      <c r="A89" s="48"/>
       <c r="B89" s="23">
         <v>40770</v>
       </c>
-      <c r="C89" s="23"/>
-      <c r="D89" s="23"/>
+      <c r="C89" s="23">
+        <v>0</v>
+      </c>
+      <c r="D89" s="23">
+        <v>0</v>
+      </c>
       <c r="E89" s="44" cm="1">
         <f t="array" aca="1" ref="E89" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C89*INDIRECT(ADDRESS(5,36)))-1</f>
         <v>0.58289376072382715</v>
@@ -4967,37 +5037,41 @@
       <c r="S92"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A93" s="50" t="s">
+      <c r="A93" s="49" t="s">
         <v>34</v>
       </c>
       <c r="B93" s="23">
         <v>40230</v>
       </c>
-      <c r="C93" s="23"/>
-      <c r="D93" s="23"/>
+      <c r="C93" s="23">
+        <v>1037.3479600000001</v>
+      </c>
+      <c r="D93" s="23">
+        <v>7287005.205844745</v>
+      </c>
       <c r="E93" s="44" cm="1">
         <f t="array" aca="1" ref="E93" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C93*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58005904310685996</v>
       </c>
       <c r="F93" s="44" cm="1">
         <f t="array" aca="1" ref="F93" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C93*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G93" s="44" t="e" cm="1">
+        <v>0.82823241744885623</v>
+      </c>
+      <c r="G93" s="44" cm="1">
         <f t="array" aca="1" ref="G93" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C93*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H93" s="44" t="e" cm="1">
+        <v>8.4777738144386312</v>
+      </c>
+      <c r="H93" s="44" cm="1">
         <f t="array" aca="1" ref="H93" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C93)*INDIRECT(ADDRESS(5,38))/(D93*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.9997599744649821</v>
       </c>
       <c r="I93" s="44" cm="1">
         <f t="array" aca="1" ref="I93" ca="1">1/((D93*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C93*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99724684572361033</v>
       </c>
       <c r="J93" s="44" cm="1">
         <f t="array" aca="1" ref="J93" ca="1">1/((D93*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C93*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99764948214528015</v>
       </c>
       <c r="L93"/>
       <c r="M93"/>
@@ -5009,35 +5083,39 @@
       <c r="S93"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A94" s="50"/>
+      <c r="A94" s="49"/>
       <c r="B94" s="23">
         <v>40240</v>
       </c>
-      <c r="C94" s="23"/>
-      <c r="D94" s="23"/>
+      <c r="C94" s="23">
+        <v>156.80258000000001</v>
+      </c>
+      <c r="D94" s="23">
+        <v>11354125.97145948</v>
+      </c>
       <c r="E94" s="44" cm="1">
         <f t="array" aca="1" ref="E94" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C94*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58246462048054126</v>
       </c>
       <c r="F94" s="44" cm="1">
         <f t="array" aca="1" ref="F94" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C94*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G94" s="44" t="e" cm="1">
+        <v>0.83212877103382366</v>
+      </c>
+      <c r="G94" s="44" cm="1">
         <f t="array" aca="1" ref="G94" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C94*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H94" s="44" t="e" cm="1">
+        <v>61.701451288297243</v>
+      </c>
+      <c r="H94" s="44" cm="1">
         <f t="array" aca="1" ref="H94" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C94)*INDIRECT(ADDRESS(5,38))/(D94*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99983529516745162</v>
       </c>
       <c r="I94" s="44" cm="1">
         <f t="array" aca="1" ref="I94" ca="1">1/((D94*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C94*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99823304166750026</v>
       </c>
       <c r="J94" s="44" cm="1">
         <f t="array" aca="1" ref="J94" ca="1">1/((D94*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C94*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99849145198521749</v>
       </c>
       <c r="L94"/>
       <c r="M94"/>
@@ -5049,35 +5127,39 @@
       <c r="S94"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A95" s="50"/>
+      <c r="A95" s="49"/>
       <c r="B95" s="23">
         <v>40250</v>
       </c>
-      <c r="C95" s="23"/>
-      <c r="D95" s="23"/>
+      <c r="C95" s="23">
+        <v>557.23129000000006</v>
+      </c>
+      <c r="D95" s="23">
+        <v>31369173.5474656</v>
+      </c>
       <c r="E95" s="44" cm="1">
         <f t="array" aca="1" ref="E95" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C95*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58136977478967555</v>
       </c>
       <c r="F95" s="44" cm="1">
         <f t="array" aca="1" ref="F95" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C95*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G95" s="44" t="e" cm="1">
+        <v>0.83035484415602356</v>
+      </c>
+      <c r="G95" s="44" cm="1">
         <f t="array" aca="1" ref="G95" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C95*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H95" s="44" t="e" cm="1">
+        <v>16.643929025861652</v>
+      </c>
+      <c r="H95" s="44" cm="1">
         <f t="array" aca="1" ref="H95" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C95)*INDIRECT(ADDRESS(5,38))/(D95*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99994213908541318</v>
       </c>
       <c r="I95" s="44" cm="1">
         <f t="array" aca="1" ref="I95" ca="1">1/((D95*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C95*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99936044606566032</v>
       </c>
       <c r="J95" s="44" cm="1">
         <f t="array" aca="1" ref="J95" ca="1">1/((D95*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C95*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99945397830733584</v>
       </c>
       <c r="L95"/>
       <c r="M95"/>
@@ -5089,12 +5171,16 @@
       <c r="S95"/>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A96" s="50"/>
+      <c r="A96" s="49"/>
       <c r="B96" s="23">
         <v>40360</v>
       </c>
-      <c r="C96" s="23"/>
-      <c r="D96" s="23"/>
+      <c r="C96" s="23">
+        <v>0</v>
+      </c>
+      <c r="D96" s="23">
+        <v>0</v>
+      </c>
       <c r="E96" s="44" cm="1">
         <f t="array" aca="1" ref="E96" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C96*INDIRECT(ADDRESS(5,36)))-1</f>
         <v>0.58289376072382715</v>
@@ -5129,35 +5215,39 @@
       <c r="S96"/>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A97" s="50"/>
+      <c r="A97" s="49"/>
       <c r="B97" s="23">
         <v>40390</v>
       </c>
-      <c r="C97" s="23"/>
-      <c r="D97" s="23"/>
+      <c r="C97" s="23">
+        <v>121.82885000000002</v>
+      </c>
+      <c r="D97" s="23">
+        <v>3863404.40287086</v>
+      </c>
       <c r="E97" s="44" cm="1">
         <f t="array" aca="1" ref="E97" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C97*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58256031707791078</v>
       </c>
       <c r="F97" s="44" cm="1">
         <f t="array" aca="1" ref="F97" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C97*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G97" s="44" t="e" cm="1">
+        <v>0.83228387036479146</v>
+      </c>
+      <c r="G97" s="44" cm="1">
         <f t="array" aca="1" ref="G97" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C97*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H97" s="44" t="e" cm="1">
+        <v>79.701322648529725</v>
+      </c>
+      <c r="H97" s="44" cm="1">
         <f t="array" aca="1" ref="H97" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C97)*INDIRECT(ADDRESS(5,38))/(D97*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99951470630275696</v>
       </c>
       <c r="I97" s="44" cm="1">
         <f t="array" aca="1" ref="I97" ca="1">1/((D97*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C97*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99480712607268296</v>
       </c>
       <c r="J97" s="44" cm="1">
         <f t="array" aca="1" ref="J97" ca="1">1/((D97*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C97*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99556655268922112</v>
       </c>
       <c r="L97"/>
       <c r="M97"/>
@@ -5169,35 +5259,39 @@
       <c r="S97"/>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A98" s="50"/>
+      <c r="A98" s="49"/>
       <c r="B98" s="23">
         <v>40710</v>
       </c>
-      <c r="C98" s="23"/>
-      <c r="D98" s="23"/>
+      <c r="C98" s="23">
+        <v>121.56012000000001</v>
+      </c>
+      <c r="D98" s="23">
+        <v>3868697.7260159361</v>
+      </c>
       <c r="E98" s="44" cm="1">
         <f t="array" aca="1" ref="E98" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C98*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58256105243309642</v>
       </c>
       <c r="F98" s="44" cm="1">
         <f t="array" aca="1" ref="F98" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C98*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G98" s="44" t="e" cm="1">
+        <v>0.83228506221360909</v>
+      </c>
+      <c r="G98" s="44" cm="1">
         <f t="array" aca="1" ref="G98" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C98*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H98" s="44" t="e" cm="1">
+        <v>79.879727099227381</v>
+      </c>
+      <c r="H98" s="44" cm="1">
         <f t="array" aca="1" ref="H98" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C98)*INDIRECT(ADDRESS(5,38))/(D98*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99951536075688052</v>
       </c>
       <c r="I98" s="44" cm="1">
         <f t="array" aca="1" ref="I98" ca="1">1/((D98*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C98*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.994814231115838</v>
       </c>
       <c r="J98" s="44" cm="1">
         <f t="array" aca="1" ref="J98" ca="1">1/((D98*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C98*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99557261869224012</v>
       </c>
       <c r="L98"/>
       <c r="M98"/>
@@ -5209,35 +5303,39 @@
       <c r="S98"/>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A99" s="50"/>
+      <c r="A99" s="49"/>
       <c r="B99" s="23">
         <v>40740</v>
       </c>
-      <c r="C99" s="23"/>
-      <c r="D99" s="23"/>
+      <c r="C99" s="23">
+        <v>204.85366000000002</v>
+      </c>
+      <c r="D99" s="23">
+        <v>79030995.547444686</v>
+      </c>
       <c r="E99" s="44" cm="1">
         <f t="array" aca="1" ref="E99" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C99*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58233315995794888</v>
       </c>
       <c r="F99" s="44" cm="1">
         <f t="array" aca="1" ref="F99" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C99*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G99" s="44" t="e" cm="1">
+        <v>0.8319157198970637</v>
+      </c>
+      <c r="G99" s="44" cm="1">
         <f t="array" aca="1" ref="G99" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C99*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H99" s="44" t="e" cm="1">
+        <v>46.994013539954963</v>
+      </c>
+      <c r="H99" s="44" cm="1">
         <f t="array" aca="1" ref="H99" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C99)*INDIRECT(ADDRESS(5,38))/(D99*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99997642094962014</v>
       </c>
       <c r="I99" s="44" cm="1">
         <f t="array" aca="1" ref="I99" ca="1">1/((D99*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C99*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99974614669089201</v>
       </c>
       <c r="J99" s="44" cm="1">
         <f t="array" aca="1" ref="J99" ca="1">1/((D99*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C99*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99978327174342818</v>
       </c>
       <c r="L99"/>
       <c r="M99"/>
@@ -5249,35 +5347,39 @@
       <c r="S99"/>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A100" s="50"/>
+      <c r="A100" s="49"/>
       <c r="B100" s="23">
         <v>40750</v>
       </c>
-      <c r="C100" s="23"/>
-      <c r="D100" s="23"/>
+      <c r="C100" s="23">
+        <v>557.19191000000001</v>
+      </c>
+      <c r="D100" s="23">
+        <v>31411483.249437507</v>
+      </c>
       <c r="E100" s="44" cm="1">
         <f t="array" aca="1" ref="E100" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C100*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58136988238734655</v>
       </c>
       <c r="F100" s="44" cm="1">
         <f t="array" aca="1" ref="F100" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C100*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G100" s="44" t="e" cm="1">
+        <v>0.83035501844324955</v>
+      </c>
+      <c r="G100" s="44" cm="1">
         <f t="array" aca="1" ref="G100" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C100*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H100" s="44" t="e" cm="1">
+        <v>16.645176025167583</v>
+      </c>
+      <c r="H100" s="44" cm="1">
         <f t="array" aca="1" ref="H100" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C100)*INDIRECT(ADDRESS(5,38))/(D100*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99994221684888895</v>
       </c>
       <c r="I100" s="44" cm="1">
         <f t="array" aca="1" ref="I100" ca="1">1/((D100*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C100*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.9993613075127854</v>
       </c>
       <c r="J100" s="44" cm="1">
         <f t="array" aca="1" ref="J100" ca="1">1/((D100*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C100*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99945471377126949</v>
       </c>
       <c r="L100"/>
       <c r="M100"/>
@@ -5289,35 +5391,39 @@
       <c r="S100"/>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A101" s="50"/>
+      <c r="A101" s="49"/>
       <c r="B101" s="23">
         <v>40760</v>
       </c>
-      <c r="C101" s="23"/>
-      <c r="D101" s="23"/>
+      <c r="C101" s="23">
+        <v>156.18735000000001</v>
+      </c>
+      <c r="D101" s="23">
+        <v>11365824.678142671</v>
+      </c>
       <c r="E101" s="44" cm="1">
         <f t="array" aca="1" ref="E101" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C101*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.58246630379885067</v>
       </c>
       <c r="F101" s="44" cm="1">
         <f t="array" aca="1" ref="F101" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C101*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G101" s="44" t="e" cm="1">
+        <v>0.83213149919082019</v>
+      </c>
+      <c r="G101" s="44" cm="1">
         <f t="array" aca="1" ref="G101" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C101*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H101" s="44" t="e" cm="1">
+        <v>61.948435527904991</v>
+      </c>
+      <c r="H101" s="44" cm="1">
         <f t="array" aca="1" ref="H101" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C101)*INDIRECT(ADDRESS(5,38))/(D101*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99983545725717204</v>
       </c>
       <c r="I101" s="44" cm="1">
         <f t="array" aca="1" ref="I101" ca="1">1/((D101*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C101*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99823486037420039</v>
       </c>
       <c r="J101" s="44" cm="1">
         <f t="array" aca="1" ref="J101" ca="1">1/((D101*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C101*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99849300471449842</v>
       </c>
       <c r="L101"/>
       <c r="M101"/>
@@ -5329,12 +5435,16 @@
       <c r="S101"/>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A102" s="50"/>
+      <c r="A102" s="49"/>
       <c r="B102" s="23">
         <v>40770</v>
       </c>
-      <c r="C102" s="23"/>
-      <c r="D102" s="23"/>
+      <c r="C102" s="23">
+        <v>0</v>
+      </c>
+      <c r="D102" s="23">
+        <v>0</v>
+      </c>
       <c r="E102" s="44" cm="1">
         <f t="array" aca="1" ref="E102" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C102*INDIRECT(ADDRESS(5,36)))-1</f>
         <v>0.58289376072382715</v>
@@ -5429,37 +5539,41 @@
       <c r="S105"/>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A106" s="50" t="s">
+      <c r="A106" s="49" t="s">
         <v>35</v>
       </c>
       <c r="B106" s="23">
         <v>40230</v>
       </c>
-      <c r="C106" s="23"/>
-      <c r="D106" s="23"/>
+      <c r="C106" s="23">
+        <v>47245.813999999998</v>
+      </c>
+      <c r="D106" s="23">
+        <v>1031090117.050784</v>
+      </c>
       <c r="E106" s="44" cm="1">
         <f t="array" aca="1" ref="E106" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C106*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.46332539962994468</v>
       </c>
       <c r="F106" s="44" cm="1">
         <f t="array" aca="1" ref="F106" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C106*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G106" s="44" t="e" cm="1">
+        <v>0.64468247975944304</v>
+      </c>
+      <c r="G106" s="44" cm="1">
         <f t="array" aca="1" ref="G106" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C106*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H106" s="44" t="e" cm="1">
+        <v>-0.79190221314105558</v>
+      </c>
+      <c r="H106" s="44" cm="1">
         <f t="array" aca="1" ref="H106" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C106)*INDIRECT(ADDRESS(5,38))/(D106*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-1.0000044625548015</v>
       </c>
       <c r="I106" s="44" cm="1">
         <f t="array" aca="1" ref="I106" ca="1">1/((D106*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C106*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.9999805426512518</v>
       </c>
       <c r="J106" s="44" cm="1">
         <f t="array" aca="1" ref="J106" ca="1">1/((D106*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C106*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99998338821242116</v>
       </c>
       <c r="L106"/>
       <c r="M106"/>
@@ -5471,35 +5585,39 @@
       <c r="S106"/>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A107" s="50"/>
+      <c r="A107" s="49"/>
       <c r="B107" s="23">
         <v>40240</v>
       </c>
-      <c r="C107" s="23"/>
-      <c r="D107" s="23"/>
+      <c r="C107" s="23">
+        <v>6705.1105000000007</v>
+      </c>
+      <c r="D107" s="23">
+        <v>626960040.28357399</v>
+      </c>
       <c r="E107" s="44" cm="1">
         <f t="array" aca="1" ref="E107" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C107*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.56474852890444538</v>
       </c>
       <c r="F107" s="44" cm="1">
         <f t="array" aca="1" ref="F107" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C107*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G107" s="44" t="e" cm="1">
+        <v>0.80354423777450745</v>
+      </c>
+      <c r="G107" s="44" cm="1">
         <f t="array" aca="1" ref="G107" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C107*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H107" s="44" t="e" cm="1">
+        <v>0.46630683144585494</v>
+      </c>
+      <c r="H107" s="44" cm="1">
         <f t="array" aca="1" ref="H107" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C107)*INDIRECT(ADDRESS(5,38))/(D107*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99999845260502773</v>
       </c>
       <c r="I107" s="44" cm="1">
         <f t="array" aca="1" ref="I107" ca="1">1/((D107*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C107*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99996800070386183</v>
       </c>
       <c r="J107" s="44" cm="1">
         <f t="array" aca="1" ref="J107" ca="1">1/((D107*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C107*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99997268047579191</v>
       </c>
       <c r="L107"/>
       <c r="M107"/>
@@ -5511,35 +5629,39 @@
       <c r="S107"/>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A108" s="50"/>
+      <c r="A108" s="49"/>
       <c r="B108" s="23">
         <v>40250</v>
       </c>
-      <c r="C108" s="23"/>
-      <c r="D108" s="23"/>
+      <c r="C108" s="23">
+        <v>71772.107000000004</v>
+      </c>
+      <c r="D108" s="23">
+        <v>1646397897.6721141</v>
+      </c>
       <c r="E108" s="44" cm="1">
         <f t="array" aca="1" ref="E108" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C108*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.40810884404929082</v>
       </c>
       <c r="F108" s="44" cm="1">
         <f t="array" aca="1" ref="F108" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C108*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G108" s="44" t="e" cm="1">
+        <v>0.56147393336645468</v>
+      </c>
+      <c r="G108" s="44" cm="1">
         <f t="array" aca="1" ref="G108" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C108*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H108" s="44" t="e" cm="1">
+        <v>-0.86301434160558599</v>
+      </c>
+      <c r="H108" s="44" cm="1">
         <f t="array" aca="1" ref="H108" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C108)*INDIRECT(ADDRESS(5,38))/(D108*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-1.0000048420309411</v>
       </c>
       <c r="I108" s="44" cm="1">
         <f t="array" aca="1" ref="I108" ca="1">1/((D108*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C108*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99998781444022278</v>
       </c>
       <c r="J108" s="44" cm="1">
         <f t="array" aca="1" ref="J108" ca="1">1/((D108*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C108*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99998959653069053</v>
       </c>
       <c r="L108"/>
       <c r="M108"/>
@@ -5551,12 +5673,16 @@
       <c r="S108"/>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A109" s="50"/>
+      <c r="A109" s="49"/>
       <c r="B109" s="23">
         <v>40360</v>
       </c>
-      <c r="C109" s="23"/>
-      <c r="D109" s="23"/>
+      <c r="C109" s="23">
+        <v>0</v>
+      </c>
+      <c r="D109" s="23">
+        <v>0</v>
+      </c>
       <c r="E109" s="44" cm="1">
         <f t="array" aca="1" ref="E109" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C109*INDIRECT(ADDRESS(5,36)))-1</f>
         <v>0.58289376072382715</v>
@@ -5591,35 +5717,39 @@
       <c r="S109"/>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A110" s="50"/>
+      <c r="A110" s="49"/>
       <c r="B110" s="23">
         <v>40390</v>
       </c>
-      <c r="C110" s="23"/>
-      <c r="D110" s="23"/>
+      <c r="C110" s="23">
+        <v>9223.4142000000011</v>
+      </c>
+      <c r="D110" s="23">
+        <v>260581404.17472795</v>
+      </c>
       <c r="E110" s="44" cm="1">
         <f t="array" aca="1" ref="E110" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C110*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.55804055021006782</v>
       </c>
       <c r="F110" s="44" cm="1">
         <f t="array" aca="1" ref="F110" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C110*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G110" s="44" t="e" cm="1">
+        <v>0.79278744201981843</v>
+      </c>
+      <c r="G110" s="44" cm="1">
         <f t="array" aca="1" ref="G110" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C110*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H110" s="44" t="e" cm="1">
+        <v>6.595552563922924E-2</v>
+      </c>
+      <c r="H110" s="44" cm="1">
         <f t="array" aca="1" ref="H110" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C110)*INDIRECT(ADDRESS(5,38))/(D110*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99999760509413094</v>
       </c>
       <c r="I110" s="44" cm="1">
         <f t="array" aca="1" ref="I110" ca="1">1/((D110*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C110*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99992300954844016</v>
       </c>
       <c r="J110" s="44" cm="1">
         <f t="array" aca="1" ref="J110" ca="1">1/((D110*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C110*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99993426910088712</v>
       </c>
       <c r="L110"/>
       <c r="M110"/>
@@ -5631,35 +5761,39 @@
       <c r="S110"/>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A111" s="50"/>
+      <c r="A111" s="49"/>
       <c r="B111" s="23">
         <v>40710</v>
       </c>
-      <c r="C111" s="23"/>
-      <c r="D111" s="23"/>
+      <c r="C111" s="23">
+        <v>8815.0568000000003</v>
+      </c>
+      <c r="D111" s="23">
+        <v>262170185.73285758</v>
+      </c>
       <c r="E111" s="44" cm="1">
         <f t="array" aca="1" ref="E111" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C111*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.55912437782218571</v>
       </c>
       <c r="F111" s="44" cm="1">
         <f t="array" aca="1" ref="F111" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C111*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G111" s="44" t="e" cm="1">
+        <v>0.79452299340709365</v>
+      </c>
+      <c r="G111" s="44" cm="1">
         <f t="array" aca="1" ref="G111" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C111*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H111" s="44" t="e" cm="1">
+        <v>0.11533590251503911</v>
+      </c>
+      <c r="H111" s="44" cm="1">
         <f t="array" aca="1" ref="H111" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C111)*INDIRECT(ADDRESS(5,38))/(D111*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99999740554820737</v>
       </c>
       <c r="I111" s="44" cm="1">
         <f t="array" aca="1" ref="I111" ca="1">1/((D111*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C111*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99992347611945365</v>
       </c>
       <c r="J111" s="44" cm="1">
         <f t="array" aca="1" ref="J111" ca="1">1/((D111*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C111*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99993466743771509</v>
       </c>
       <c r="L111"/>
       <c r="M111"/>
@@ -5671,35 +5805,39 @@
       <c r="S111"/>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A112" s="50"/>
+      <c r="A112" s="49"/>
       <c r="B112" s="23">
         <v>40740</v>
       </c>
-      <c r="C112" s="23"/>
-      <c r="D112" s="23"/>
+      <c r="C112" s="23">
+        <v>217563.06000000003</v>
+      </c>
+      <c r="D112" s="23">
+        <v>4291188796.0038123</v>
+      </c>
       <c r="E112" s="44" cm="1">
         <f t="array" aca="1" ref="E112" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C112*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.15013489900632693</v>
       </c>
       <c r="F112" s="44" cm="1">
         <f t="array" aca="1" ref="F112" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C112*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G112" s="44" t="e" cm="1">
+        <v>0.2004547201692275</v>
+      </c>
+      <c r="G112" s="44" cm="1">
         <f t="array" aca="1" ref="G112" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C112*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H112" s="44" t="e" cm="1">
+        <v>-0.95480965687948438</v>
+      </c>
+      <c r="H112" s="44" cm="1">
         <f t="array" aca="1" ref="H112" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C112)*INDIRECT(ADDRESS(5,38))/(D112*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-1.0000065268048766</v>
       </c>
       <c r="I112" s="44" cm="1">
         <f t="array" aca="1" ref="I112" ca="1">1/((D112*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C112*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99999532477340114</v>
       </c>
       <c r="J112" s="44" cm="1">
         <f t="array" aca="1" ref="J112" ca="1">1/((D112*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C112*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99999600850700954</v>
       </c>
       <c r="L112"/>
       <c r="M112"/>
@@ -5711,35 +5849,39 @@
       <c r="S112"/>
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A113" s="50"/>
+      <c r="A113" s="49"/>
       <c r="B113" s="23">
         <v>40750</v>
       </c>
-      <c r="C113" s="23"/>
-      <c r="D113" s="23"/>
+      <c r="C113" s="23">
+        <v>67977.899000000005</v>
+      </c>
+      <c r="D113" s="23">
+        <v>1538722208.1181324</v>
+      </c>
       <c r="E113" s="44" cm="1">
         <f t="array" aca="1" ref="E113" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C113*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.41637676695530668</v>
       </c>
       <c r="F113" s="44" cm="1">
         <f t="array" aca="1" ref="F113" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C113*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G113" s="44" t="e" cm="1">
+        <v>0.57379142474431521</v>
+      </c>
+      <c r="G113" s="44" cm="1">
         <f t="array" aca="1" ref="G113" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C113*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H113" s="44" t="e" cm="1">
+        <v>-0.85536844362092845</v>
+      </c>
+      <c r="H113" s="44" cm="1">
         <f t="array" aca="1" ref="H113" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C113)*INDIRECT(ADDRESS(5,38))/(D113*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-1.000004841989631</v>
       </c>
       <c r="I113" s="44" cm="1">
         <f t="array" aca="1" ref="I113" ca="1">1/((D113*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C113*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99998696172714396</v>
       </c>
       <c r="J113" s="44" cm="1">
         <f t="array" aca="1" ref="J113" ca="1">1/((D113*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C113*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99998886852356506</v>
       </c>
       <c r="L113"/>
       <c r="M113"/>
@@ -5751,35 +5893,39 @@
       <c r="S113"/>
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A114" s="50"/>
+      <c r="A114" s="49"/>
       <c r="B114" s="23">
         <v>40760</v>
       </c>
-      <c r="C114" s="23"/>
-      <c r="D114" s="23"/>
+      <c r="C114" s="23">
+        <v>6460.9974000000002</v>
+      </c>
+      <c r="D114" s="23">
+        <v>615179576.38995016</v>
+      </c>
       <c r="E114" s="44" cm="1">
         <f t="array" aca="1" ref="E114" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C114*INDIRECT(ADDRESS(5,36)))-1</f>
-        <v>0.58289376072382715</v>
+        <v>0.56540184256753823</v>
       </c>
       <c r="F114" s="44" cm="1">
         <f t="array" aca="1" ref="F114" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,24))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C114*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>0.83282435452232617</v>
-      </c>
-      <c r="G114" s="44" t="e" cm="1">
+        <v>0.80459382024606541</v>
+      </c>
+      <c r="G114" s="44" cm="1">
         <f t="array" aca="1" ref="G114" ca="1">INDIRECT(ADDRESS(5,35))/((1-INDIRECT(ADDRESS(5,33)))*C114*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H114" s="44" t="e" cm="1">
+        <v>0.52170767500221116</v>
+      </c>
+      <c r="H114" s="44" cm="1">
         <f t="array" aca="1" ref="H114" ca="1">(INDIRECT(ADDRESS(5,35))-(1-INDIRECT(ADDRESS(5,33)))*C114)*INDIRECT(ADDRESS(5,38))/(D114*INDIRECT(ADDRESS(5,37)))-1</f>
-        <v>#DIV/0!</v>
+        <v>-0.99999836843912371</v>
       </c>
       <c r="I114" s="44" cm="1">
         <f t="array" aca="1" ref="I114" ca="1">1/((D114*INDIRECT(ADDRESS(5,36))/INDIRECT(ADDRESS(5,25))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C114*INDIRECT(ADDRESS(5,36)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,23)))^2)^0.5 - 1</f>
-        <v>0.58289376072382715</v>
+        <v>-0.99996738792904438</v>
       </c>
       <c r="J114" s="44" cm="1">
         <f t="array" aca="1" ref="J114" ca="1">1/((D114*INDIRECT(ADDRESS(5,37))/INDIRECT(ADDRESS(5,26))/INDIRECT(ADDRESS(5,32)))^2+((INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C114*INDIRECT(ADDRESS(5,37)))/INDIRECT(ADDRESS(5,32))/INDIRECT(ADDRESS(5,24)))^2)^0.5 - 1</f>
-        <v>0.83282435452232617</v>
+        <v>-0.99997215731689526</v>
       </c>
       <c r="L114"/>
       <c r="M114"/>
@@ -5791,12 +5937,16 @@
       <c r="S114"/>
     </row>
     <row r="115" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A115" s="50"/>
+      <c r="A115" s="49"/>
       <c r="B115" s="23">
         <v>40770</v>
       </c>
-      <c r="C115" s="23"/>
-      <c r="D115" s="23"/>
+      <c r="C115" s="23">
+        <v>0</v>
+      </c>
+      <c r="D115" s="23">
+        <v>0</v>
+      </c>
       <c r="E115" s="44" cm="1">
         <f t="array" aca="1" ref="E115" ca="1">INDIRECT(ADDRESS(5,32))*INDIRECT(ADDRESS(5,23))/(INDIRECT(ADDRESS(5,34))+INDIRECT(ADDRESS(5,33))*C115*INDIRECT(ADDRESS(5,36)))-1</f>
         <v>0.58289376072382715</v>
@@ -6627,7 +6777,7 @@
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A159" s="46" t="s">
+      <c r="A159" s="50" t="s">
         <v>30</v>
       </c>
       <c r="B159" s="35">
@@ -6652,7 +6802,7 @@
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A160" s="46"/>
+      <c r="A160" s="50"/>
       <c r="B160" s="35">
         <v>40240</v>
       </c>
@@ -6675,7 +6825,7 @@
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A161" s="46"/>
+      <c r="A161" s="50"/>
       <c r="B161" s="35">
         <v>40250</v>
       </c>
@@ -6698,7 +6848,7 @@
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A162" s="46"/>
+      <c r="A162" s="50"/>
       <c r="B162" s="35">
         <v>40360</v>
       </c>
@@ -6712,7 +6862,7 @@
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A163" s="46"/>
+      <c r="A163" s="50"/>
       <c r="B163" s="35">
         <v>40390</v>
       </c>
@@ -6735,7 +6885,7 @@
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A164" s="46"/>
+      <c r="A164" s="50"/>
       <c r="B164" s="35">
         <v>40710</v>
       </c>
@@ -6758,7 +6908,7 @@
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A165" s="46"/>
+      <c r="A165" s="50"/>
       <c r="B165" s="35">
         <v>40740</v>
       </c>
@@ -6781,7 +6931,7 @@
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A166" s="46"/>
+      <c r="A166" s="50"/>
       <c r="B166" s="35">
         <v>40750</v>
       </c>
@@ -6804,7 +6954,7 @@
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A167" s="46"/>
+      <c r="A167" s="50"/>
       <c r="B167" s="35">
         <v>40760</v>
       </c>
@@ -6827,7 +6977,7 @@
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A168" s="46"/>
+      <c r="A168" s="50"/>
       <c r="B168" s="35">
         <v>40770</v>
       </c>
@@ -6858,7 +7008,7 @@
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A170" s="46" t="s">
+      <c r="A170" s="50" t="s">
         <v>31</v>
       </c>
       <c r="B170" s="35">
@@ -6883,7 +7033,7 @@
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A171" s="46"/>
+      <c r="A171" s="50"/>
       <c r="B171" s="35">
         <v>40240</v>
       </c>
@@ -6906,7 +7056,7 @@
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A172" s="46"/>
+      <c r="A172" s="50"/>
       <c r="B172" s="35">
         <v>40250</v>
       </c>
@@ -6929,7 +7079,7 @@
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A173" s="46"/>
+      <c r="A173" s="50"/>
       <c r="B173" s="35">
         <v>40360</v>
       </c>
@@ -6946,7 +7096,7 @@
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A174" s="46"/>
+      <c r="A174" s="50"/>
       <c r="B174" s="35">
         <v>40390</v>
       </c>
@@ -6969,7 +7119,7 @@
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A175" s="46"/>
+      <c r="A175" s="50"/>
       <c r="B175" s="35">
         <v>40710</v>
       </c>
@@ -6992,7 +7142,7 @@
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A176" s="46"/>
+      <c r="A176" s="50"/>
       <c r="B176" s="35">
         <v>40740</v>
       </c>
@@ -7015,7 +7165,7 @@
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A177" s="46"/>
+      <c r="A177" s="50"/>
       <c r="B177" s="35">
         <v>40750</v>
       </c>
@@ -7038,7 +7188,7 @@
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A178" s="46"/>
+      <c r="A178" s="50"/>
       <c r="B178" s="35">
         <v>40760</v>
       </c>
@@ -7061,7 +7211,7 @@
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A179" s="46"/>
+      <c r="A179" s="50"/>
       <c r="B179" s="35">
         <v>40770</v>
       </c>
@@ -7092,7 +7242,7 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A181" s="46" t="s">
+      <c r="A181" s="50" t="s">
         <v>32</v>
       </c>
       <c r="B181" s="35">
@@ -7117,7 +7267,7 @@
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A182" s="46"/>
+      <c r="A182" s="50"/>
       <c r="B182" s="35">
         <v>40240</v>
       </c>
@@ -7140,7 +7290,7 @@
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A183" s="46"/>
+      <c r="A183" s="50"/>
       <c r="B183" s="35">
         <v>40250</v>
       </c>
@@ -7163,7 +7313,7 @@
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A184" s="46"/>
+      <c r="A184" s="50"/>
       <c r="B184" s="35">
         <v>40360</v>
       </c>
@@ -7179,7 +7329,7 @@
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A185" s="46"/>
+      <c r="A185" s="50"/>
       <c r="B185" s="35">
         <v>40390</v>
       </c>
@@ -7202,7 +7352,7 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A186" s="46"/>
+      <c r="A186" s="50"/>
       <c r="B186" s="35">
         <v>40710</v>
       </c>
@@ -7225,7 +7375,7 @@
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A187" s="46"/>
+      <c r="A187" s="50"/>
       <c r="B187" s="35">
         <v>40740</v>
       </c>
@@ -7248,7 +7398,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A188" s="46"/>
+      <c r="A188" s="50"/>
       <c r="B188" s="35">
         <v>40750</v>
       </c>
@@ -7271,7 +7421,7 @@
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A189" s="46"/>
+      <c r="A189" s="50"/>
       <c r="B189" s="35">
         <v>40760</v>
       </c>
@@ -7294,7 +7444,7 @@
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A190" s="46"/>
+      <c r="A190" s="50"/>
       <c r="B190" s="35">
         <v>40770</v>
       </c>
@@ -7325,62 +7475,81 @@
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A192" s="47" t="s">
-        <v>33</v>
+      <c r="A192" s="46" t="s">
+        <v>60</v>
       </c>
       <c r="B192" s="35">
         <v>40230</v>
       </c>
-      <c r="C192" s="9"/>
-      <c r="E192" s="45"/>
+      <c r="C192" s="39">
+        <v>688.53740000000005</v>
+      </c>
+      <c r="D192" s="39">
+        <v>57.630740000000003</v>
+      </c>
+      <c r="E192" s="39">
+        <v>4.5427759999999999</v>
+      </c>
       <c r="F192" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>757.39114000000006</v>
       </c>
       <c r="G192" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3676.1329074071541</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A193" s="48"/>
+      <c r="A193" s="47"/>
       <c r="B193" s="35">
         <v>40240</v>
       </c>
-      <c r="C193" s="9"/>
-      <c r="E193" s="45"/>
+      <c r="C193" s="39">
+        <v>49.77919</v>
+      </c>
+      <c r="D193" s="39">
+        <v>16.450189999999999</v>
+      </c>
+      <c r="E193" s="39">
+        <v>5685.7830000000004</v>
+      </c>
       <c r="F193" s="26">
         <f t="shared" ref="F193:F223" si="4">C193*1.1*1</f>
-        <v>0</v>
+        <v>54.757109000000007</v>
       </c>
       <c r="G193" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>35561238.825024046</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A194" s="48"/>
+      <c r="A194" s="47"/>
       <c r="B194" s="35">
         <v>40250</v>
       </c>
-      <c r="C194" s="9"/>
-      <c r="E194" s="45"/>
+      <c r="C194" s="39">
+        <v>127.52670000000001</v>
+      </c>
+      <c r="D194" s="39">
+        <v>3186.0210000000002</v>
+      </c>
+      <c r="E194" s="39">
+        <v>8010.116</v>
+      </c>
       <c r="F194" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>140.27937000000003</v>
       </c>
       <c r="G194" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>81743956.96048671</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A195" s="48"/>
+      <c r="A195" s="47"/>
       <c r="B195" s="35">
         <v>40360</v>
       </c>
-      <c r="C195" s="9"/>
-      <c r="E195" s="45"/>
       <c r="F195" s="26">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -7391,87 +7560,122 @@
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A196" s="48"/>
+      <c r="A196" s="47"/>
       <c r="B196" s="35">
         <v>40390</v>
       </c>
-      <c r="C196" s="9"/>
-      <c r="E196" s="45"/>
+      <c r="C196" s="39">
+        <v>143.64150000000001</v>
+      </c>
+      <c r="D196" s="39">
+        <v>1504.145</v>
+      </c>
+      <c r="E196" s="39">
+        <v>308.87490000000003</v>
+      </c>
       <c r="F196" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>158.00565000000003</v>
       </c>
       <c r="G196" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2593641.473362511</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A197" s="48"/>
+      <c r="A197" s="47"/>
       <c r="B197" s="35">
         <v>40710</v>
       </c>
-      <c r="C197" s="9"/>
-      <c r="E197" s="45"/>
+      <c r="C197" s="39">
+        <v>143.45699999999999</v>
+      </c>
+      <c r="D197" s="39">
+        <v>1505.5440000000001</v>
+      </c>
+      <c r="E197" s="39">
+        <v>307.92329999999998</v>
+      </c>
       <c r="F197" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>157.80270000000002</v>
       </c>
       <c r="G197" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2597627.4440807798</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A198" s="48"/>
+      <c r="A198" s="47"/>
       <c r="B198" s="35">
         <v>40740</v>
       </c>
-      <c r="C198" s="9"/>
-      <c r="E198" s="45"/>
+      <c r="C198" s="39">
+        <v>734.20240000000001</v>
+      </c>
+      <c r="D198" s="39">
+        <v>10138.93</v>
+      </c>
+      <c r="E198" s="39">
+        <v>213.05889999999999</v>
+      </c>
       <c r="F198" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>807.62264000000005</v>
       </c>
       <c r="G198" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>113127625.20374614</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A199" s="48"/>
+      <c r="A199" s="47"/>
       <c r="B199" s="35">
         <v>40750</v>
       </c>
-      <c r="C199" s="9"/>
-      <c r="E199" s="45"/>
+      <c r="C199" s="39">
+        <v>127.3843</v>
+      </c>
+      <c r="D199" s="39">
+        <v>3190.915</v>
+      </c>
+      <c r="E199" s="39">
+        <v>8013.9719999999998</v>
+      </c>
       <c r="F199" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>140.12273000000002</v>
       </c>
       <c r="G199" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>81846254.329409897</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A200" s="48"/>
+      <c r="A200" s="47"/>
       <c r="B200" s="35">
         <v>40760</v>
       </c>
-      <c r="C200" s="9"/>
-      <c r="E200" s="45"/>
+      <c r="C200" s="39">
+        <v>49.574950000000001</v>
+      </c>
+      <c r="D200" s="39">
+        <v>16.539090000000002</v>
+      </c>
+      <c r="E200" s="39">
+        <v>5688.4449999999997</v>
+      </c>
       <c r="F200" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>54.532445000000003</v>
       </c>
       <c r="G200" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>35594548.06547533</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A201" s="49"/>
+      <c r="A201" s="48"/>
       <c r="B201" s="35">
         <v>40770</v>
       </c>
@@ -7502,57 +7706,78 @@
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A203" s="50" t="s">
-        <v>34</v>
+      <c r="A203" s="49" t="s">
+        <v>59</v>
       </c>
       <c r="B203" s="35">
         <v>40230</v>
       </c>
-      <c r="C203" s="9"/>
-      <c r="E203" s="45"/>
+      <c r="C203" s="39">
+        <v>943.04359999999997</v>
+      </c>
+      <c r="D203" s="39">
+        <v>54.833159999999999</v>
+      </c>
+      <c r="E203" s="39">
+        <v>2573.2359999999999</v>
+      </c>
       <c r="F203" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1037.3479600000001</v>
       </c>
       <c r="G203" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7287005.205844745</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A204" s="50"/>
+      <c r="A204" s="49"/>
       <c r="B204" s="35">
         <v>40240</v>
       </c>
-      <c r="C204" s="9"/>
-      <c r="E204" s="45"/>
+      <c r="C204" s="39">
+        <v>142.5478</v>
+      </c>
+      <c r="D204" s="39">
+        <v>50.66272</v>
+      </c>
+      <c r="E204" s="39">
+        <v>3212.377</v>
+      </c>
       <c r="F204" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156.80258000000001</v>
       </c>
       <c r="G204" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11354125.97145948</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A205" s="50"/>
+      <c r="A205" s="49"/>
       <c r="B205" s="35">
         <v>40250</v>
       </c>
-      <c r="C205" s="9"/>
-      <c r="E205" s="45"/>
+      <c r="C205" s="39">
+        <v>506.57389999999998</v>
+      </c>
+      <c r="D205" s="39">
+        <v>2215.2199999999998</v>
+      </c>
+      <c r="E205" s="39">
+        <v>4859.0360000000001</v>
+      </c>
       <c r="F205" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>557.23129000000006</v>
       </c>
       <c r="G205" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>31369173.5474656</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A206" s="50"/>
+      <c r="A206" s="49"/>
       <c r="B206" s="35">
         <v>40360</v>
       </c>
@@ -7568,87 +7793,122 @@
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A207" s="50"/>
+      <c r="A207" s="49"/>
       <c r="B207" s="35">
         <v>40390</v>
       </c>
-      <c r="C207" s="9"/>
-      <c r="E207" s="45"/>
+      <c r="C207" s="39">
+        <v>110.7535</v>
+      </c>
+      <c r="D207" s="39">
+        <v>1867.88</v>
+      </c>
+      <c r="E207" s="39">
+        <v>152.34870000000001</v>
+      </c>
       <c r="F207" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>121.82885000000002</v>
       </c>
       <c r="G207" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3863404.40287086</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A208" s="50"/>
+      <c r="A208" s="49"/>
       <c r="B208" s="35">
         <v>40710</v>
       </c>
-      <c r="C208" s="9"/>
-      <c r="E208" s="45"/>
+      <c r="C208" s="39">
+        <v>110.50920000000001</v>
+      </c>
+      <c r="D208" s="39">
+        <v>1869.204</v>
+      </c>
+      <c r="E208" s="39">
+        <v>151.9024</v>
+      </c>
       <c r="F208" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>121.56012000000001</v>
       </c>
       <c r="G208" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3868697.7260159361</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A209" s="50"/>
+      <c r="A209" s="49"/>
       <c r="B209" s="35">
         <v>40740</v>
       </c>
-      <c r="C209" s="9"/>
-      <c r="E209" s="45"/>
+      <c r="C209" s="39">
+        <v>186.23060000000001</v>
+      </c>
+      <c r="D209" s="39">
+        <v>8475.0159999999996</v>
+      </c>
+      <c r="E209" s="39">
+        <v>143.05029999999999</v>
+      </c>
       <c r="F209" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>204.85366000000002</v>
       </c>
       <c r="G209" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>79030995.547444686</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A210" s="50"/>
+      <c r="A210" s="49"/>
       <c r="B210" s="35">
         <v>40750</v>
       </c>
-      <c r="C210" s="9"/>
-      <c r="E210" s="45"/>
+      <c r="C210" s="39">
+        <v>506.53809999999999</v>
+      </c>
+      <c r="D210" s="39">
+        <v>2217.6579999999999</v>
+      </c>
+      <c r="E210" s="39">
+        <v>4861.8810000000003</v>
+      </c>
       <c r="F210" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>557.19191000000001</v>
       </c>
       <c r="G210" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>31411483.249437507</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A211" s="50"/>
+      <c r="A211" s="49"/>
       <c r="B211" s="35">
         <v>40760</v>
       </c>
-      <c r="C211" s="9"/>
-      <c r="E211" s="45"/>
+      <c r="C211" s="39">
+        <v>141.98849999999999</v>
+      </c>
+      <c r="D211" s="39">
+        <v>50.466900000000003</v>
+      </c>
+      <c r="E211" s="39">
+        <v>3214.0349999999999</v>
+      </c>
       <c r="F211" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>156.18735000000001</v>
       </c>
       <c r="G211" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>11365824.678142671</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A212" s="50"/>
+      <c r="A212" s="49"/>
       <c r="B212" s="35">
         <v>40770</v>
       </c>
@@ -7679,57 +7939,78 @@
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A214" s="50" t="s">
-        <v>35</v>
+      <c r="A214" s="49" t="s">
+        <v>58</v>
       </c>
       <c r="B214" s="35">
         <v>40230</v>
       </c>
-      <c r="C214" s="9"/>
-      <c r="E214" s="45"/>
+      <c r="C214" s="39">
+        <v>42950.74</v>
+      </c>
+      <c r="D214" s="39">
+        <v>30326.57</v>
+      </c>
+      <c r="E214" s="39">
+        <v>4201.643</v>
+      </c>
       <c r="F214" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>47245.813999999998</v>
       </c>
       <c r="G214" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1031090117.050784</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A215" s="50"/>
+      <c r="A215" s="49"/>
       <c r="B215" s="35">
         <v>40240</v>
       </c>
-      <c r="C215" s="9"/>
-      <c r="E215" s="45"/>
+      <c r="C215" s="39">
+        <v>6095.5550000000003</v>
+      </c>
+      <c r="D215" s="39">
+        <v>23865.65</v>
+      </c>
+      <c r="E215" s="39">
+        <v>628.03110000000004</v>
+      </c>
       <c r="F215" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6705.1105000000007</v>
       </c>
       <c r="G215" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>626960040.28357399</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A216" s="50"/>
+      <c r="A216" s="49"/>
       <c r="B216" s="35">
         <v>40250</v>
       </c>
-      <c r="C216" s="9"/>
-      <c r="E216" s="45"/>
+      <c r="C216" s="39">
+        <v>65247.37</v>
+      </c>
+      <c r="D216" s="39">
+        <v>38590.81</v>
+      </c>
+      <c r="E216" s="39">
+        <v>2733.998</v>
+      </c>
       <c r="F216" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>71772.107000000004</v>
       </c>
       <c r="G216" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1646397897.6721141</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A217" s="50"/>
+      <c r="A217" s="49"/>
       <c r="B217" s="35">
         <v>40360</v>
       </c>
@@ -7745,87 +8026,122 @@
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A218" s="50"/>
+      <c r="A218" s="49"/>
       <c r="B218" s="35">
         <v>40390</v>
       </c>
-      <c r="C218" s="9"/>
-      <c r="E218" s="45"/>
+      <c r="C218" s="39">
+        <v>8384.9220000000005</v>
+      </c>
+      <c r="D218" s="39">
+        <v>6226.7330000000002</v>
+      </c>
+      <c r="E218" s="39">
+        <v>14075.51</v>
+      </c>
       <c r="F218" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>9223.4142000000011</v>
       </c>
       <c r="G218" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>260581404.17472795</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A219" s="50"/>
+      <c r="A219" s="49"/>
       <c r="B219" s="35">
         <v>40710</v>
       </c>
-      <c r="C219" s="9"/>
-      <c r="E219" s="45"/>
+      <c r="C219" s="39">
+        <v>8013.6880000000001</v>
+      </c>
+      <c r="D219" s="39">
+        <v>5733.8959999999997</v>
+      </c>
+      <c r="E219" s="39">
+        <v>14333.84</v>
+      </c>
       <c r="F219" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8815.0568000000003</v>
       </c>
       <c r="G219" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>262170185.73285758</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A220" s="50"/>
+      <c r="A220" s="49"/>
       <c r="B220" s="35">
         <v>40740</v>
       </c>
-      <c r="C220" s="9"/>
-      <c r="E220" s="45"/>
+      <c r="C220" s="39">
+        <v>197784.6</v>
+      </c>
+      <c r="D220" s="39">
+        <v>712.327</v>
+      </c>
+      <c r="E220" s="39">
+        <v>62454.57</v>
+      </c>
       <c r="F220" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>217563.06000000003</v>
       </c>
       <c r="G220" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4291188796.0038123</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A221" s="50"/>
+      <c r="A221" s="49"/>
       <c r="B221" s="35">
         <v>40750</v>
       </c>
-      <c r="C221" s="9"/>
-      <c r="E221" s="45"/>
+      <c r="C221" s="39">
+        <v>61798.09</v>
+      </c>
+      <c r="D221" s="39">
+        <v>37282.39</v>
+      </c>
+      <c r="E221" s="39">
+        <v>2976.8719999999998</v>
+      </c>
       <c r="F221" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>67977.899000000005</v>
       </c>
       <c r="G221" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1538722208.1181324</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A222" s="50"/>
+      <c r="A222" s="49"/>
       <c r="B222" s="35">
         <v>40760</v>
       </c>
-      <c r="C222" s="9"/>
-      <c r="E222" s="45"/>
+      <c r="C222" s="39">
+        <v>5873.634</v>
+      </c>
+      <c r="D222" s="39">
+        <v>23645.040000000001</v>
+      </c>
+      <c r="E222" s="39">
+        <v>407.73</v>
+      </c>
       <c r="F222" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6460.9974000000002</v>
       </c>
       <c r="G222" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>615179576.38995016</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A223" s="50"/>
+      <c r="A223" s="49"/>
       <c r="B223" s="35">
         <v>40770</v>
       </c>
@@ -7842,17 +8158,20 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="L80:L82"/>
-    <mergeCell ref="L83:L88"/>
-    <mergeCell ref="A106:A115"/>
-    <mergeCell ref="A67:A76"/>
-    <mergeCell ref="A54:A63"/>
-    <mergeCell ref="A93:A102"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="A28:A37"/>
-    <mergeCell ref="A41:A50"/>
-    <mergeCell ref="A80:A89"/>
+    <mergeCell ref="A181:A190"/>
+    <mergeCell ref="A192:A201"/>
+    <mergeCell ref="A203:A212"/>
+    <mergeCell ref="A214:A223"/>
+    <mergeCell ref="A128:A137"/>
+    <mergeCell ref="A138:A147"/>
+    <mergeCell ref="A148:A157"/>
+    <mergeCell ref="A159:A168"/>
+    <mergeCell ref="A170:A179"/>
+    <mergeCell ref="M80:M82"/>
+    <mergeCell ref="M83:M85"/>
+    <mergeCell ref="M86:M88"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="N79:O79"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="L41:L43"/>
     <mergeCell ref="L44:L49"/>
@@ -7864,28 +8183,25 @@
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="L2:L4"/>
     <mergeCell ref="L5:L10"/>
-    <mergeCell ref="M80:M82"/>
-    <mergeCell ref="M83:M85"/>
-    <mergeCell ref="M86:M88"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="N79:O79"/>
-    <mergeCell ref="A181:A190"/>
-    <mergeCell ref="A192:A201"/>
-    <mergeCell ref="A203:A212"/>
-    <mergeCell ref="A214:A223"/>
-    <mergeCell ref="A128:A137"/>
-    <mergeCell ref="A138:A147"/>
-    <mergeCell ref="A148:A157"/>
-    <mergeCell ref="A159:A168"/>
-    <mergeCell ref="A170:A179"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="A28:A37"/>
+    <mergeCell ref="A41:A50"/>
+    <mergeCell ref="A80:A89"/>
+    <mergeCell ref="L80:L82"/>
+    <mergeCell ref="L83:L88"/>
+    <mergeCell ref="A106:A115"/>
+    <mergeCell ref="A67:A76"/>
+    <mergeCell ref="A54:A63"/>
+    <mergeCell ref="A93:A102"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:J158 E163:E168 E159:E161 F159:J168 E169:J1048576">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+  <conditionalFormatting sqref="E1:J158 E163:E168 E159:E161 F159:J168 E169:J194 E202:J1048576 E196:E201 F195:J201">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:S1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>